<commit_message>
Update localization files for various languages with corrections and improvements in translations, including adjustments to lead type descriptions and QR code messages.
</commit_message>
<xml_diff>
--- a/Multilanguage_Client_live_editing_sheet.xlsx
+++ b/Multilanguage_Client_live_editing_sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4930840E-1D16-4E2F-922E-C1D91036F780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{375CF3AF-C260-44AC-91BD-C2E843212903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="FrontendMissing Punjabi Content" sheetId="2" r:id="rId2"/>
     <sheet name="Ic-app-text" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -932,22 +932,22 @@
     <t>லீட் வகை</t>
   </si>
   <si>
-    <t>ലീഡ് തരം</t>
+    <t>വീടിന്റെ തരം</t>
   </si>
   <si>
     <t>ಲೀಡ್ ನ ಪ್ರಕಾರ</t>
   </si>
   <si>
-    <t xml:space="preserve">ଲିଡ ର ପ୍ରକାର </t>
-  </si>
-  <si>
-    <t>ਲੀਡ ਦੀ ਕਿਸਮ</t>
-  </si>
-  <si>
-    <t>લીડનો પ્રકાર</t>
-  </si>
-  <si>
-    <t>লীডৰ ধৰণ</t>
+    <t>ଘର ପ୍ରକାର</t>
+  </si>
+  <si>
+    <t>ਘਰ ਦੀ ਕਿਸਮ</t>
+  </si>
+  <si>
+    <t>ઘરનો પ્રકાર</t>
+  </si>
+  <si>
+    <t>ঘৰৰ ধৰণ</t>
   </si>
   <si>
     <t>projectDetails/requirement</t>
@@ -10861,7 +10861,7 @@
     <t>કૃપા કરીને વોરંટી બંધ કરવા માટે ગ્રાહકને મોકલવામાં આવેલ OTP દાખલ કરો.</t>
   </si>
   <si>
-    <t>অনুগ্ৰহ কৰি ৱাৰেণ্টী বন্ধ কৰাৰ বাবে গ্ৰাহকলৈ প্ৰেৰণ কৰা OTP প্ৰৱেশ কৰক</t>
+    <t>অনুগ্ৰহ কৰি প্ৰকল্পটো বন্ধ কৰাৰ বাবে গ্ৰাহকলৈ প্ৰেৰণ কৰা অ'.টি.পি প্ৰৱেশ কৰক</t>
   </si>
   <si>
     <t>warranty/certifiedContractorsOnly</t>
@@ -11077,7 +11077,7 @@
     <t>વોટરપ્રૂફિંગ સ્કેન કરેલ વિસ્તાર</t>
   </si>
   <si>
-    <t>Waterproofing স্কেন কৰা ঠাই</t>
+    <t>ৱাটাৰপ্ৰুফিং স্কেন কৰা ঠাই</t>
   </si>
   <si>
     <t>warranty/paintablescannedpercentage</t>
@@ -11149,7 +11149,7 @@
     <t>વોટરપ્રૂફિંગ સ્કેન કરેલ ટકાવારી</t>
   </si>
   <si>
-    <t>Waterproofing স্কেন কৰা শতাংশ</t>
+    <t>ৱাটাৰপ্ৰুফিং স্কেন কৰা শতাংশ</t>
   </si>
   <si>
     <t>projectDetails/productTagSuccessMessage</t>
@@ -13999,7 +13999,7 @@
     <t>ଏକ OTP ପଠାଯାଇଛି</t>
   </si>
   <si>
-    <t>એક OTP મોકલવામાં આવ્યો છે</t>
+    <t>એક ઓટીપી મોકલવામાં આવ્યો છે</t>
   </si>
   <si>
     <t>এটা অ’টিপি প্ৰেৰণ কৰা হৈছে</t>
@@ -37931,28 +37931,7 @@
     <t>ଆପଣଙ୍କୁ ରେଫର୍ କରାଯାଇଛି</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">તમને </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">____ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>એ રેફર કર્યા છે</t>
-    </r>
+    <t>તમને એ રેફર કર્યા છે</t>
   </si>
   <si>
     <t>আপোনাক যি ৰেফাৰ কৰিছিল</t>
@@ -45068,30 +45047,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t xml:space="preserve">ક્યુઆર કોડની મુદ્દત </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">___ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>ના રોજ વીતી ગઈ</t>
-    </r>
+    <t>ક્યુઆર કોડની મુદ્દત ના રોજ વીતી ગઈ</t>
   </si>
   <si>
     <r>
@@ -49082,7 +49038,7 @@
     <t>તમે આ ક્યુ.આર. કોડ પહેલાથી જ સ્કેન કરી લીધો છે</t>
   </si>
   <si>
-    <t>আপুনি ইতিমধ্যে এই QR ক'ডটো স্কেন কৰিছে</t>
+    <t>আপুনি ইতিমধ্যে এই কিউ.আৰ ক'ডটো স্কেন কৰিছে</t>
   </si>
   <si>
     <t>earningerrors/dbvalidationdetail</t>
@@ -49118,7 +49074,7 @@
     <t>કૃપા કરીને તમારી ટ્રાન્ઝેક્શન હિસ્ટ્રી તપાસો અથવા વધુ વિગતો માટે તમારા ટી.એસ.એમ સાથે વાત કરો</t>
   </si>
   <si>
-    <t>অনুগ্ৰহ কৰি আপোনাৰ লেনদেনৰ ইতিহাস পৰীক্ষা কৰক বা অধিক বিৱৰণৰ বাবে আপোনাৰ TSM ৰ সৈতে কথা পাতক</t>
+    <t>অনুগ্ৰহ কৰি আপোনাৰ লেনদেনৰ ইতিহাস পৰীক্ষা কৰক বা অধিক বিৱৰণৰ বাবে আপোনাৰ টি.এচ.এম ৰ সৈতে কথা পাতক</t>
   </si>
   <si>
     <t>earningerrors/invalidloyalty</t>
@@ -49209,7 +49165,7 @@
     <t>અમે અમારા રેકોર્ડમાં આ ક્યુ.આર. કોડ શોધી શક્યા નથી. વધુ સહાય માટે કૃપા કરીને તમારા ટી.એસ.એમ ને ક્યુ.આર. કોડનો ફોટો મોકલો.</t>
   </si>
   <si>
-    <t>আমি আমাৰ ৰেকৰ্ডত এই QR ক'ডটো বিচাৰি উলিয়াব পৰা নাই। অধিক সহায়ৰ বাবে অনুগ্ৰহ কৰি QR ক'ডৰ এখন ছবি আপোনাৰ TSM লৈ প্ৰেৰণ কৰক।</t>
+    <t>আমি আমাৰ ৰেকৰ্ডত এই কিউ.আৰ ক'ডটো বিচাৰি উলিয়াব পৰা নাই। অধিক সহায়ৰ বাবে অনুগ্ৰহ কৰি কিউ.আৰ ক'ডৰ এখন ছবি আপোনাৰ টি.এচ.এম লৈ প্ৰেৰণ কৰক।</t>
   </si>
   <si>
     <t>earningerrors/backendissue</t>
@@ -49986,8 +49942,7 @@
     <t>કે.વાય.સી. વિગતો</t>
   </si>
   <si>
-    <t>KYC
- সবিশেষ</t>
+    <t>কে.ৱাই.চি\n সবিশেষ</t>
   </si>
   <si>
     <t>profilecompletion/yourteam</t>
@@ -50116,7 +50071,7 @@
     <t>કે.વાય.સી. પર જાઓ</t>
   </si>
   <si>
-    <t>KYC লৈ যাওক</t>
+    <t>কে.ৱাই.চি লৈ যাওক</t>
   </si>
   <si>
     <t>kycpopup/pandetails</t>
@@ -50188,7 +50143,7 @@
     <t>તમારું કે.વાય.સી. પૂર્ણ કરો</t>
   </si>
   <si>
-    <t>আপোনাৰ KYC সম্পূৰ্ণ কৰক</t>
+    <t>আপোনাৰ কে.ৱাই.চি সম্পূৰ্ণ কৰক</t>
   </si>
   <si>
     <t>kycpopup/profiledetailrequired</t>
@@ -50368,7 +50323,7 @@
     <t>જો પાન વિગતો આપવામાં ન આવે તો કલમ 194R મુજબ 20% ટી.ડી.એસ. લાગુ પડે છે.</t>
   </si>
   <si>
-    <t>20% TDS ধাৰা 198আৰ অনুসৰি প্ৰযোজ্য হ’ব যদিহে পেনৰ সবিশেষ প্ৰদান কৰা নহয়।</t>
+    <t>20% টি.ডি.এছ ধাৰা 198আৰ অনুসৰি প্ৰযোজ্য হ’ব যদিহে পেনৰ সবিশেষ প্ৰদান কৰা নহয়।</t>
   </si>
   <si>
     <t>redemptionnotavailable</t>
@@ -50548,7 +50503,7 @@
     <t>ટી.ડી.એસ. (સ્રોત પર કર કપાત)</t>
   </si>
   <si>
-    <t>TDS (উৎসত কৰ্তন কৰা কৰ)</t>
+    <t>টি.ডি.এছ (উৎসত কৰ্তন কৰা কৰ)</t>
   </si>
   <si>
     <t>redemerrorpoint</t>
@@ -53351,8 +53306,8 @@
   <dimension ref="A1:X685"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="K495" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M499" sqref="M499"/>
+      <pane ySplit="1" topLeftCell="I15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>

</xml_diff>